<commit_message>
Stuff we did together when brainstorming lol
</commit_message>
<xml_diff>
--- a/To-Do/MainALR.xlsx
+++ b/To-Do/MainALR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmcdonnell1\Downloads\Cost-of-Betrayal\To-Do\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529F3C6C-29BA-40F0-ACB7-F91410C07AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550BD3C8-7B1D-48E7-807A-3961D275175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42696" yWindow="144" windowWidth="17880" windowHeight="15348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="84">
   <si>
     <t>MAIN ALR</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>status and nothing else!</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Dialogue Backend</t>
@@ -249,12 +246,42 @@
   <si>
     <t>This node wipes all of the player's data and returns them to the title screen if they aren't already there, allowing the player to clear a save slot if needed, this node also has an artificial delay that can be changed if needed</t>
   </si>
+  <si>
+    <t>Tumbleweed Model</t>
+  </si>
+  <si>
+    <t>This'll be used in A LOT of places, it needs to look good</t>
+  </si>
+  <si>
+    <t>Save Slot UI</t>
+  </si>
+  <si>
+    <t>UI_Saving</t>
+  </si>
+  <si>
+    <t>I'm going to use this same UI for the loading page too don't worry lol</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/media?url=https%3A%2F%2Fpreview.redd.it%2Ffile-softlocked-in-black-void-due-to-bug-v0-6c484dtpekne1.jpg%3Fwidth%3D1080%26crop%3Dsmart%26auto%3Dwebp%26s%3D464ff43c8e532a3e7fd476df9249248f2237f309</t>
+  </si>
+  <si>
+    <t>Settings UI</t>
+  </si>
+  <si>
+    <t>UI_Settings</t>
+  </si>
+  <si>
+    <t>NGL mostly gonna be an empty outline and I'll add in all the settings stuff when making the UI function</t>
+  </si>
+  <si>
+    <t>idk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -280,6 +307,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -503,10 +537,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -551,8 +586,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
@@ -1115,7 +1152,7 @@
   </sheetPr>
   <dimension ref="A1:AM1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1354,20 +1391,20 @@
       <c r="B8" s="17"/>
       <c r="C8" s="3"/>
       <c r="D8" s="7" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
       <c r="H8" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="17"/>
       <c r="K8" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="17"/>
@@ -1402,17 +1439,17 @@
         <v>12</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
       <c r="H9" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="17"/>
       <c r="K9" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="17"/>
@@ -1444,20 +1481,20 @@
     </row>
     <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
       <c r="H10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
       <c r="K10" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="17"/>
@@ -1492,17 +1529,17 @@
         <v>12</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
       <c r="H11" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
       <c r="K11" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="17"/>
@@ -1537,17 +1574,17 @@
         <v>12</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
       <c r="H12" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="17"/>
       <c r="K12" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="17"/>
@@ -1582,17 +1619,17 @@
         <v>12</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
       <c r="H13" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="17"/>
       <c r="K13" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L13" s="16"/>
       <c r="M13" s="17"/>
@@ -6413,7 +6450,7 @@
   <dimension ref="A1:AR1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6430,7 +6467,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -6438,7 +6475,7 @@
     <row r="2" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -6468,7 +6505,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
@@ -6483,7 +6520,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="17"/>
       <c r="N5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O5" s="16"/>
       <c r="P5" s="17"/>
@@ -6492,7 +6529,7 @@
         <v>7</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T5" s="16"/>
       <c r="U5" s="17"/>
@@ -6507,7 +6544,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="17"/>
       <c r="AB5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC5" s="16"/>
       <c r="AD5" s="17"/>
@@ -6515,7 +6552,7 @@
         <v>7</v>
       </c>
       <c r="AG5" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AH5" s="20"/>
       <c r="AI5" s="21"/>
@@ -6530,7 +6567,7 @@
       <c r="AN5" s="16"/>
       <c r="AO5" s="17"/>
       <c r="AP5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AQ5" s="16"/>
       <c r="AR5" s="17"/>
@@ -6544,17 +6581,17 @@
         <v>12</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
       <c r="H6" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="17"/>
       <c r="K6" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" s="16"/>
       <c r="M6" s="17"/>
@@ -6596,17 +6633,17 @@
       <c r="B7" s="17"/>
       <c r="D7" s="7"/>
       <c r="E7" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
       <c r="H7" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="17"/>
       <c r="K7" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="17"/>
@@ -6648,17 +6685,17 @@
       <c r="B8" s="17"/>
       <c r="D8" s="7"/>
       <c r="E8" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
       <c r="H8" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="17"/>
       <c r="K8" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="17"/>
@@ -6696,17 +6733,17 @@
     <row r="9" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="7"/>
       <c r="E9" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
       <c r="H9" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="17"/>
       <c r="K9" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="17"/>
@@ -6744,17 +6781,17 @@
     <row r="10" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="7"/>
       <c r="E10" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
       <c r="H10" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
       <c r="K10" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="17"/>
@@ -6791,22 +6828,22 @@
     </row>
     <row r="11" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="7"/>
       <c r="E11" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
       <c r="H11" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
       <c r="K11" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="17"/>
@@ -6843,13 +6880,19 @@
     </row>
     <row r="12" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="7"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>74</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="15"/>
+      <c r="H12" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="I12" s="16"/>
       <c r="J12" s="17"/>
-      <c r="K12" s="15"/>
+      <c r="K12" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="L12" s="16"/>
       <c r="M12" s="17"/>
       <c r="N12" s="15"/>
@@ -6969,7 +7012,7 @@
     </row>
     <row r="15" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3"/>
       <c r="D15" s="7"/>
@@ -10810,6 +10853,10 @@
     <mergeCell ref="S70:U70"/>
     <mergeCell ref="V70:X70"/>
     <mergeCell ref="Y70:AA70"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="K73:M73"/>
     <mergeCell ref="AB71:AD71"/>
     <mergeCell ref="AG71:AI71"/>
     <mergeCell ref="AJ71:AL71"/>
@@ -10822,14 +10869,6 @@
     <mergeCell ref="S71:U71"/>
     <mergeCell ref="V71:X71"/>
     <mergeCell ref="Y71:AA71"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="K80:M80"/>
-    <mergeCell ref="N80:P80"/>
-    <mergeCell ref="S80:U80"/>
-    <mergeCell ref="V80:X80"/>
-    <mergeCell ref="Y80:AA80"/>
     <mergeCell ref="AB72:AD72"/>
     <mergeCell ref="AG72:AI72"/>
     <mergeCell ref="AJ72:AL72"/>
@@ -10871,10 +10910,6 @@
     <mergeCell ref="S10:U10"/>
     <mergeCell ref="V10:X10"/>
     <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="K73:M73"/>
     <mergeCell ref="N73:P73"/>
     <mergeCell ref="S73:U73"/>
     <mergeCell ref="V73:X73"/>
@@ -10884,6 +10919,21 @@
     <mergeCell ref="AJ81:AL81"/>
     <mergeCell ref="AM81:AO81"/>
     <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AJ80:AL80"/>
+    <mergeCell ref="AM80:AO80"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AJ74:AL74"/>
+    <mergeCell ref="AM74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AJ76:AL76"/>
+    <mergeCell ref="AM76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AJ78:AL78"/>
+    <mergeCell ref="AM78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AP80:AR80"/>
     <mergeCell ref="E81:G81"/>
     <mergeCell ref="H81:J81"/>
     <mergeCell ref="K81:M81"/>
@@ -10893,9 +10943,13 @@
     <mergeCell ref="Y81:AA81"/>
     <mergeCell ref="AB80:AD80"/>
     <mergeCell ref="AG80:AI80"/>
-    <mergeCell ref="AJ80:AL80"/>
-    <mergeCell ref="AM80:AO80"/>
-    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="H80:J80"/>
+    <mergeCell ref="K80:M80"/>
+    <mergeCell ref="N80:P80"/>
+    <mergeCell ref="S80:U80"/>
+    <mergeCell ref="V80:X80"/>
+    <mergeCell ref="Y80:AA80"/>
     <mergeCell ref="E75:G75"/>
     <mergeCell ref="H75:J75"/>
     <mergeCell ref="K75:M75"/>
@@ -10905,9 +10959,6 @@
     <mergeCell ref="Y75:AA75"/>
     <mergeCell ref="AB74:AD74"/>
     <mergeCell ref="AG74:AI74"/>
-    <mergeCell ref="AJ74:AL74"/>
-    <mergeCell ref="AM74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
     <mergeCell ref="E74:G74"/>
     <mergeCell ref="H74:J74"/>
     <mergeCell ref="K74:M74"/>
@@ -10915,7 +10966,6 @@
     <mergeCell ref="S74:U74"/>
     <mergeCell ref="V74:X74"/>
     <mergeCell ref="Y74:AA74"/>
-    <mergeCell ref="AP77:AR77"/>
     <mergeCell ref="E77:G77"/>
     <mergeCell ref="H77:J77"/>
     <mergeCell ref="K77:M77"/>
@@ -10925,9 +10975,6 @@
     <mergeCell ref="Y77:AA77"/>
     <mergeCell ref="AB76:AD76"/>
     <mergeCell ref="AG76:AI76"/>
-    <mergeCell ref="AJ76:AL76"/>
-    <mergeCell ref="AM76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
     <mergeCell ref="E76:G76"/>
     <mergeCell ref="H76:J76"/>
     <mergeCell ref="K76:M76"/>
@@ -10935,7 +10982,6 @@
     <mergeCell ref="S76:U76"/>
     <mergeCell ref="V76:X76"/>
     <mergeCell ref="Y76:AA76"/>
-    <mergeCell ref="AP79:AR79"/>
     <mergeCell ref="E79:G79"/>
     <mergeCell ref="H79:J79"/>
     <mergeCell ref="K79:M79"/>
@@ -10945,9 +10991,6 @@
     <mergeCell ref="Y79:AA79"/>
     <mergeCell ref="AB78:AD78"/>
     <mergeCell ref="AG78:AI78"/>
-    <mergeCell ref="AJ78:AL78"/>
-    <mergeCell ref="AM78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
     <mergeCell ref="E78:G78"/>
     <mergeCell ref="H78:J78"/>
     <mergeCell ref="K78:M78"/>
@@ -11618,8 +11661,8 @@
   </sheetPr>
   <dimension ref="A1:AR1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:P8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11636,7 +11679,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -11644,7 +11687,7 @@
     <row r="2" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -11674,7 +11717,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
@@ -11689,7 +11732,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="17"/>
       <c r="N5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O5" s="16"/>
       <c r="P5" s="17"/>
@@ -11698,7 +11741,7 @@
         <v>7</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T5" s="16"/>
       <c r="U5" s="17"/>
@@ -11713,7 +11756,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="17"/>
       <c r="AB5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC5" s="16"/>
       <c r="AD5" s="17"/>
@@ -11721,7 +11764,7 @@
         <v>7</v>
       </c>
       <c r="AG5" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AH5" s="20"/>
       <c r="AI5" s="21"/>
@@ -11736,7 +11779,7 @@
       <c r="AN5" s="16"/>
       <c r="AO5" s="17"/>
       <c r="AP5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AQ5" s="16"/>
       <c r="AR5" s="17"/>
@@ -11748,22 +11791,22 @@
       <c r="B6" s="17"/>
       <c r="D6" s="7"/>
       <c r="E6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
       <c r="H6" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="17"/>
       <c r="K6" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L6" s="16"/>
       <c r="M6" s="17"/>
       <c r="N6" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O6" s="16"/>
       <c r="P6" s="17"/>
@@ -11802,22 +11845,22 @@
       <c r="B7" s="17"/>
       <c r="D7" s="7"/>
       <c r="E7" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
       <c r="H7" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="17"/>
       <c r="K7" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="17"/>
       <c r="N7" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O7" s="16"/>
       <c r="P7" s="17"/>
@@ -11856,22 +11899,22 @@
       <c r="B8" s="17"/>
       <c r="D8" s="7"/>
       <c r="E8" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
       <c r="H8" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="17"/>
       <c r="K8" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="17"/>
       <c r="N8" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O8" s="16"/>
       <c r="P8" s="17"/>
@@ -11905,16 +11948,24 @@
     </row>
     <row r="9" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="7"/>
-      <c r="E9" s="25"/>
+      <c r="E9" s="25" t="s">
+        <v>76</v>
+      </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="25"/>
+      <c r="H9" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="I9" s="16"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="25"/>
+      <c r="K9" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="L9" s="16"/>
       <c r="M9" s="17"/>
-      <c r="N9" s="25"/>
+      <c r="N9" s="38" t="s">
+        <v>79</v>
+      </c>
       <c r="O9" s="16"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="2"/>
@@ -11947,16 +11998,24 @@
     </row>
     <row r="10" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="7"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>80</v>
+      </c>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="15"/>
+      <c r="H10" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
-      <c r="K10" s="15"/>
+      <c r="K10" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="L10" s="16"/>
       <c r="M10" s="17"/>
-      <c r="N10" s="15"/>
+      <c r="N10" s="15" t="s">
+        <v>83</v>
+      </c>
       <c r="O10" s="16"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="2"/>
@@ -11989,7 +12048,7 @@
     </row>
     <row r="11" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="7"/>
@@ -12161,7 +12220,7 @@
     </row>
     <row r="15" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3"/>
       <c r="D15" s="7"/>
@@ -16002,6 +16061,10 @@
     <mergeCell ref="S70:U70"/>
     <mergeCell ref="V70:X70"/>
     <mergeCell ref="Y70:AA70"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="K73:M73"/>
     <mergeCell ref="AB71:AD71"/>
     <mergeCell ref="AG71:AI71"/>
     <mergeCell ref="AJ71:AL71"/>
@@ -16014,14 +16077,6 @@
     <mergeCell ref="S71:U71"/>
     <mergeCell ref="V71:X71"/>
     <mergeCell ref="Y71:AA71"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="K80:M80"/>
-    <mergeCell ref="N80:P80"/>
-    <mergeCell ref="S80:U80"/>
-    <mergeCell ref="V80:X80"/>
-    <mergeCell ref="Y80:AA80"/>
     <mergeCell ref="AB72:AD72"/>
     <mergeCell ref="AG72:AI72"/>
     <mergeCell ref="AJ72:AL72"/>
@@ -16063,10 +16118,6 @@
     <mergeCell ref="S10:U10"/>
     <mergeCell ref="V10:X10"/>
     <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="K73:M73"/>
     <mergeCell ref="N73:P73"/>
     <mergeCell ref="S73:U73"/>
     <mergeCell ref="V73:X73"/>
@@ -16076,6 +16127,21 @@
     <mergeCell ref="AJ81:AL81"/>
     <mergeCell ref="AM81:AO81"/>
     <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AJ80:AL80"/>
+    <mergeCell ref="AM80:AO80"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AJ74:AL74"/>
+    <mergeCell ref="AM74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AJ76:AL76"/>
+    <mergeCell ref="AM76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AJ78:AL78"/>
+    <mergeCell ref="AM78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AP80:AR80"/>
     <mergeCell ref="E81:G81"/>
     <mergeCell ref="H81:J81"/>
     <mergeCell ref="K81:M81"/>
@@ -16085,9 +16151,13 @@
     <mergeCell ref="Y81:AA81"/>
     <mergeCell ref="AB80:AD80"/>
     <mergeCell ref="AG80:AI80"/>
-    <mergeCell ref="AJ80:AL80"/>
-    <mergeCell ref="AM80:AO80"/>
-    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="H80:J80"/>
+    <mergeCell ref="K80:M80"/>
+    <mergeCell ref="N80:P80"/>
+    <mergeCell ref="S80:U80"/>
+    <mergeCell ref="V80:X80"/>
+    <mergeCell ref="Y80:AA80"/>
     <mergeCell ref="E75:G75"/>
     <mergeCell ref="H75:J75"/>
     <mergeCell ref="K75:M75"/>
@@ -16097,9 +16167,6 @@
     <mergeCell ref="Y75:AA75"/>
     <mergeCell ref="AB74:AD74"/>
     <mergeCell ref="AG74:AI74"/>
-    <mergeCell ref="AJ74:AL74"/>
-    <mergeCell ref="AM74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
     <mergeCell ref="E74:G74"/>
     <mergeCell ref="H74:J74"/>
     <mergeCell ref="K74:M74"/>
@@ -16107,7 +16174,6 @@
     <mergeCell ref="S74:U74"/>
     <mergeCell ref="V74:X74"/>
     <mergeCell ref="Y74:AA74"/>
-    <mergeCell ref="AP77:AR77"/>
     <mergeCell ref="E77:G77"/>
     <mergeCell ref="H77:J77"/>
     <mergeCell ref="K77:M77"/>
@@ -16117,9 +16183,6 @@
     <mergeCell ref="Y77:AA77"/>
     <mergeCell ref="AB76:AD76"/>
     <mergeCell ref="AG76:AI76"/>
-    <mergeCell ref="AJ76:AL76"/>
-    <mergeCell ref="AM76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
     <mergeCell ref="E76:G76"/>
     <mergeCell ref="H76:J76"/>
     <mergeCell ref="K76:M76"/>
@@ -16127,7 +16190,6 @@
     <mergeCell ref="S76:U76"/>
     <mergeCell ref="V76:X76"/>
     <mergeCell ref="Y76:AA76"/>
-    <mergeCell ref="AP79:AR79"/>
     <mergeCell ref="E79:G79"/>
     <mergeCell ref="H79:J79"/>
     <mergeCell ref="K79:M79"/>
@@ -16137,9 +16199,6 @@
     <mergeCell ref="Y79:AA79"/>
     <mergeCell ref="AB78:AD78"/>
     <mergeCell ref="AG78:AI78"/>
-    <mergeCell ref="AJ78:AL78"/>
-    <mergeCell ref="AM78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
     <mergeCell ref="E78:G78"/>
     <mergeCell ref="H78:J78"/>
     <mergeCell ref="K78:M78"/>
@@ -16793,12 +16852,15 @@
       <formula1>"In Progress,Blocked,Finished"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N9" r:id="rId1" xr:uid="{F2467E79-6640-4084-9FCB-035D8962D55B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -16810,7 +16872,9 @@
   </sheetPr>
   <dimension ref="A1:AR1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16826,7 +16890,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -16834,7 +16898,7 @@
     <row r="2" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -16864,7 +16928,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
@@ -16879,7 +16943,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="17"/>
       <c r="N5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O5" s="16"/>
       <c r="P5" s="17"/>
@@ -16888,7 +16952,7 @@
         <v>7</v>
       </c>
       <c r="S5" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T5" s="16"/>
       <c r="U5" s="17"/>
@@ -16903,7 +16967,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="17"/>
       <c r="AB5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC5" s="16"/>
       <c r="AD5" s="17"/>
@@ -16911,7 +16975,7 @@
         <v>7</v>
       </c>
       <c r="AG5" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AH5" s="20"/>
       <c r="AI5" s="21"/>
@@ -16926,7 +16990,7 @@
       <c r="AN5" s="16"/>
       <c r="AO5" s="17"/>
       <c r="AP5" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AQ5" s="16"/>
       <c r="AR5" s="17"/>
@@ -17155,7 +17219,7 @@
     </row>
     <row r="11" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="7"/>
@@ -17327,7 +17391,7 @@
     </row>
     <row r="15" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3"/>
       <c r="D15" s="7"/>
@@ -21168,6 +21232,10 @@
     <mergeCell ref="S70:U70"/>
     <mergeCell ref="V70:X70"/>
     <mergeCell ref="Y70:AA70"/>
+    <mergeCell ref="AP73:AR73"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="K73:M73"/>
     <mergeCell ref="AB71:AD71"/>
     <mergeCell ref="AG71:AI71"/>
     <mergeCell ref="AJ71:AL71"/>
@@ -21180,14 +21248,6 @@
     <mergeCell ref="S71:U71"/>
     <mergeCell ref="V71:X71"/>
     <mergeCell ref="Y71:AA71"/>
-    <mergeCell ref="AP80:AR80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="K80:M80"/>
-    <mergeCell ref="N80:P80"/>
-    <mergeCell ref="S80:U80"/>
-    <mergeCell ref="V80:X80"/>
-    <mergeCell ref="Y80:AA80"/>
     <mergeCell ref="AB72:AD72"/>
     <mergeCell ref="AG72:AI72"/>
     <mergeCell ref="AJ72:AL72"/>
@@ -21229,10 +21289,6 @@
     <mergeCell ref="S10:U10"/>
     <mergeCell ref="V10:X10"/>
     <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="AP73:AR73"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="K73:M73"/>
     <mergeCell ref="N73:P73"/>
     <mergeCell ref="S73:U73"/>
     <mergeCell ref="V73:X73"/>
@@ -21242,6 +21298,21 @@
     <mergeCell ref="AJ81:AL81"/>
     <mergeCell ref="AM81:AO81"/>
     <mergeCell ref="AP81:AR81"/>
+    <mergeCell ref="AJ80:AL80"/>
+    <mergeCell ref="AM80:AO80"/>
+    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="AJ74:AL74"/>
+    <mergeCell ref="AM74:AO74"/>
+    <mergeCell ref="AP74:AR74"/>
+    <mergeCell ref="AP77:AR77"/>
+    <mergeCell ref="AJ76:AL76"/>
+    <mergeCell ref="AM76:AO76"/>
+    <mergeCell ref="AP76:AR76"/>
+    <mergeCell ref="AP79:AR79"/>
+    <mergeCell ref="AJ78:AL78"/>
+    <mergeCell ref="AM78:AO78"/>
+    <mergeCell ref="AP78:AR78"/>
+    <mergeCell ref="AP80:AR80"/>
     <mergeCell ref="E81:G81"/>
     <mergeCell ref="H81:J81"/>
     <mergeCell ref="K81:M81"/>
@@ -21251,9 +21322,13 @@
     <mergeCell ref="Y81:AA81"/>
     <mergeCell ref="AB80:AD80"/>
     <mergeCell ref="AG80:AI80"/>
-    <mergeCell ref="AJ80:AL80"/>
-    <mergeCell ref="AM80:AO80"/>
-    <mergeCell ref="AP75:AR75"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="H80:J80"/>
+    <mergeCell ref="K80:M80"/>
+    <mergeCell ref="N80:P80"/>
+    <mergeCell ref="S80:U80"/>
+    <mergeCell ref="V80:X80"/>
+    <mergeCell ref="Y80:AA80"/>
     <mergeCell ref="E75:G75"/>
     <mergeCell ref="H75:J75"/>
     <mergeCell ref="K75:M75"/>
@@ -21263,9 +21338,6 @@
     <mergeCell ref="Y75:AA75"/>
     <mergeCell ref="AB74:AD74"/>
     <mergeCell ref="AG74:AI74"/>
-    <mergeCell ref="AJ74:AL74"/>
-    <mergeCell ref="AM74:AO74"/>
-    <mergeCell ref="AP74:AR74"/>
     <mergeCell ref="E74:G74"/>
     <mergeCell ref="H74:J74"/>
     <mergeCell ref="K74:M74"/>
@@ -21273,7 +21345,6 @@
     <mergeCell ref="S74:U74"/>
     <mergeCell ref="V74:X74"/>
     <mergeCell ref="Y74:AA74"/>
-    <mergeCell ref="AP77:AR77"/>
     <mergeCell ref="E77:G77"/>
     <mergeCell ref="H77:J77"/>
     <mergeCell ref="K77:M77"/>
@@ -21283,9 +21354,6 @@
     <mergeCell ref="Y77:AA77"/>
     <mergeCell ref="AB76:AD76"/>
     <mergeCell ref="AG76:AI76"/>
-    <mergeCell ref="AJ76:AL76"/>
-    <mergeCell ref="AM76:AO76"/>
-    <mergeCell ref="AP76:AR76"/>
     <mergeCell ref="E76:G76"/>
     <mergeCell ref="H76:J76"/>
     <mergeCell ref="K76:M76"/>
@@ -21293,7 +21361,6 @@
     <mergeCell ref="S76:U76"/>
     <mergeCell ref="V76:X76"/>
     <mergeCell ref="Y76:AA76"/>
-    <mergeCell ref="AP79:AR79"/>
     <mergeCell ref="E79:G79"/>
     <mergeCell ref="H79:J79"/>
     <mergeCell ref="K79:M79"/>
@@ -21303,9 +21370,6 @@
     <mergeCell ref="Y79:AA79"/>
     <mergeCell ref="AB78:AD78"/>
     <mergeCell ref="AG78:AI78"/>
-    <mergeCell ref="AJ78:AL78"/>
-    <mergeCell ref="AM78:AO78"/>
-    <mergeCell ref="AP78:AR78"/>
     <mergeCell ref="E78:G78"/>
     <mergeCell ref="H78:J78"/>
     <mergeCell ref="K78:M78"/>

</xml_diff>

<commit_message>
Interp done for LDT
finished the Interp Point tool for the Level Design Toolkit
</commit_message>
<xml_diff>
--- a/To-Do/MainALR.xlsx
+++ b/To-Do/MainALR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmcdonnell1\Downloads\Cost-of-Betrayal\To-Do\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB33F30-6B54-4BE8-A543-4EDE0131A39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167519F8-05AB-4A12-B493-FE0E0ECB6DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42696" yWindow="144" windowWidth="17880" windowHeight="15348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="131">
   <si>
     <t>MainALR</t>
   </si>
@@ -425,6 +425,12 @@
   </si>
   <si>
     <t>Level Design Toolkit: A blueprint that allows the level designer to select and object, set it to a certain point, and then interpolate that object between that set position and another selected position without needing to touch any blueprints, should only be used for basic movements, any advanced animation should use a specified blueprint</t>
+  </si>
+  <si>
+    <t>Title Button UI</t>
+  </si>
+  <si>
+    <t>Yony u alr know gng</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1347,7 @@
   <dimension ref="A1:AM1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20:M20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2074,7 +2080,7 @@
     </row>
     <row r="19" spans="4:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D19" s="8" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>126</v>
@@ -11907,8 +11913,8 @@
   </sheetPr>
   <dimension ref="A1:AR1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:G6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12145,7 +12151,9 @@
         <v>82</v>
       </c>
       <c r="B8" s="17"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" s="42" t="s">
         <v>83</v>
       </c>
@@ -12501,14 +12509,22 @@
         <v>66</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>129</v>
+      </c>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
+      <c r="H15" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="I15" s="16"/>
       <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
+      <c r="K15" s="18" t="s">
+        <v>130</v>
+      </c>
       <c r="L15" s="16"/>
       <c r="M15" s="17"/>
       <c r="N15" s="18"/>

</xml_diff>